<commit_message>
Pagina principal, planificacion y css actualizados
</commit_message>
<xml_diff>
--- a/Planificacion/Planificacion.xlsx
+++ b/Planificacion/Planificacion.xlsx
@@ -80,9 +80,6 @@
     <t xml:space="preserve"> - Mostrar todos los recursos desde consultas.</t>
   </si>
   <si>
-    <t xml:space="preserve"> - AL clicar en el recurso se redirigirá al detalle.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> - Formulario para filtrar</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t xml:space="preserve"> - Repasar la página</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Al clicar en el recurso se redirigirá al detalle.</t>
   </si>
 </sst>
 </file>
@@ -238,68 +238,68 @@
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -617,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,334 +628,334 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="F7" s="3" t="s">
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="F7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="5"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="14"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="8"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="17"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="17"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="11"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15"/>
-      <c r="F10" s="13" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="F10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="15"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
-      <c r="F11" s="16" t="s">
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="F11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="18"/>
-      <c r="F12" s="16" t="s">
+      <c r="C12" s="7"/>
+      <c r="D12" s="8"/>
+      <c r="F12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="18"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="18"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="18"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="8"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="18"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="18"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="21"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="21"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="11"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
     </row>
     <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5"/>
-      <c r="F19" s="3" t="s">
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+      <c r="F19" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="5"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="14"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="8"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="17"/>
     </row>
     <row r="21" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="9"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="11"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="11"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="20"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="20"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="15"/>
-      <c r="F22" s="13" t="s">
+      <c r="C22" s="4"/>
+      <c r="D22" s="5"/>
+      <c r="F22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G22" s="14"/>
-      <c r="H22" s="15"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="5"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8"/>
+      <c r="F23" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="17"/>
-      <c r="D23" s="18"/>
-      <c r="F23" s="16" t="s">
+      <c r="G23" s="7"/>
+      <c r="H23" s="8"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="8"/>
+      <c r="F24" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="8"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="8"/>
+      <c r="F25" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="18"/>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="16"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="18"/>
-      <c r="F24" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24" s="17"/>
-      <c r="H24" s="18"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="16"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="18"/>
-      <c r="F25" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G25" s="17"/>
-      <c r="H25" s="18"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="8"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="16"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="18"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="18"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="8"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="8"/>
     </row>
     <row r="27" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="19"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="21"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="21"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="11"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="11"/>
     </row>
     <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="5"/>
-      <c r="F29" s="3" t="s">
+      <c r="C29" s="13"/>
+      <c r="D29" s="14"/>
+      <c r="F29" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G29" s="4"/>
-      <c r="H29" s="5"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="14"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="6"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="8"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="8"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="17"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="17"/>
     </row>
     <row r="31" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="9"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="11"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="11"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="20"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="20"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="5"/>
+      <c r="F32" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G32" s="4"/>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="15"/>
-      <c r="F32" s="13" t="s">
+      <c r="C33" s="7"/>
+      <c r="D33" s="8"/>
+      <c r="F33" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="G32" s="14"/>
-      <c r="H32" s="15"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="16" t="s">
+      <c r="G33" s="7"/>
+      <c r="H33" s="8"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="17"/>
-      <c r="D33" s="18"/>
-      <c r="F33" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="G33" s="17"/>
-      <c r="H33" s="18"/>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C34" s="17"/>
-      <c r="D34" s="18"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="18"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="8"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="8"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="16"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="18"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="18"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="8"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="8"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="16"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="18"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="18"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="8"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="8"/>
     </row>
     <row r="37" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="19"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="21"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="21"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="11"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>